<commit_message>
avances en el cuaderno final. Implementacion de heatmaps y posicion promedio con listas desplegables.
</commit_message>
<xml_diff>
--- a/ChatGPT+ aportes/Diccionario de terminos partido - jugador.xlsx
+++ b/ChatGPT+ aportes/Diccionario de terminos partido - jugador.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alvaro\Proyectos\Proyecto Gronestats\GroneStats\ChatGPT+ aportes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6BED24F-7147-4DC9-96CA-F5C98B9B65F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F56FC5F6-7003-401D-A6FA-E5967654E0CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{72D1DFFF-6DF8-43EC-B76F-11990B5C98B9}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$B$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$D$92</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Hoja2!$B$2:$D$47</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="139">
   <si>
     <t>ID_Estadistica_Jugador</t>
   </si>
@@ -416,6 +416,48 @@
   </si>
   <si>
     <t>Duelos Aereos Ganados Totales</t>
+  </si>
+  <si>
+    <t>Faltas Cometidas Totales</t>
+  </si>
+  <si>
+    <t>Goles esperados del equipo</t>
+  </si>
+  <si>
+    <t>Grandes Oportunidades Falladas Totales</t>
+  </si>
+  <si>
+    <t>ARQUERO-02</t>
+  </si>
+  <si>
+    <t>Pases totales</t>
+  </si>
+  <si>
+    <t>Pases Acertados del equipo</t>
+  </si>
+  <si>
+    <t>VOLANTE-01</t>
+  </si>
+  <si>
+    <t>Tiros Bloqueados Totales</t>
+  </si>
+  <si>
+    <t>Tiros fuera totales</t>
+  </si>
+  <si>
+    <t>Balones Largos Acertados Totales</t>
+  </si>
+  <si>
+    <t>Centros Acertados Totales</t>
+  </si>
+  <si>
+    <t>Contiendas Totales</t>
+  </si>
+  <si>
+    <t>Pases Intentados</t>
+  </si>
+  <si>
+    <t>Tiros al Arco del jugador</t>
   </si>
 </sst>
 </file>
@@ -515,6 +557,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8B5E4525-6500-49D7-870C-9E21117AA188}" name="Diccionario" displayName="Diccionario" ref="A1:E93" totalsRowShown="0">
+  <autoFilter ref="A1:E93" xr:uid="{8B5E4525-6500-49D7-870C-9E21117AA188}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E93">
+    <sortCondition ref="A1:A93"/>
+  </sortState>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{EF87B0E1-9C1E-4E0E-BF56-0985B323C725}" name="Estadistica_Global"/>
+    <tableColumn id="2" xr3:uid="{AF777CC1-3216-484C-AC02-3015A8959883}" name="ID_Estadistica_JUGADOR_Global"/>
+    <tableColumn id="3" xr3:uid="{8E981479-7417-48BB-AB7F-7BDE2CD9E9D8}" name="ID_Estadistica_Partido"/>
+    <tableColumn id="4" xr3:uid="{E3585C8A-C9F3-4AB7-8B90-8920F0CEC7C9}" name="ID_Estadistica_Jugador"/>
+    <tableColumn id="5" xr3:uid="{431CE225-77EC-4B85-BFEF-BC9F47ED82CF}" name="Tipo_Estadistica"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -814,18 +873,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E37CA9D-18F6-44B6-95D3-67168C9C737D}">
-  <dimension ref="A1:E91"/>
+  <dimension ref="A1:E93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="34.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.6640625" customWidth="1"/>
-    <col min="3" max="3" width="30.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.21875" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" customWidth="1"/>
+    <col min="5" max="5" width="30.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -836,20 +896,23 @@
         <v>110</v>
       </c>
       <c r="C1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
         <v>118</v>
-      </c>
-      <c r="D1" t="s">
-        <v>109</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>73</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B2">
+        <v>23</v>
+      </c>
+      <c r="E2" t="s">
         <v>117</v>
       </c>
     </row>
@@ -857,1343 +920,1265 @@
       <c r="A3" t="s">
         <v>69</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B3">
+        <v>24</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
         <v>117</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C4" t="s">
-        <v>116</v>
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
       </c>
       <c r="D4">
-        <v>22</v>
+        <f>VLOOKUP(A4,Hoja3!$F$3:$G$45,2,0)</f>
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>113</v>
-      </c>
-      <c r="E5">
-        <f>VLOOKUP(A5,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>2</v>
+        <v>112</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>114</v>
-      </c>
-      <c r="C6" t="s">
-        <v>120</v>
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>75</v>
       </c>
       <c r="D6">
-        <v>17</v>
+        <f>VLOOKUP(A6,Hoja3!$F$3:$G$45,2,0)</f>
+        <v>4</v>
+      </c>
+      <c r="E6" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>119</v>
-      </c>
-      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>25</v>
+      </c>
+      <c r="D7">
         <f>VLOOKUP(A7,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>115</v>
-      </c>
-      <c r="C8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
         <v>116</v>
-      </c>
-      <c r="D8">
-        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" t="s">
-        <v>117</v>
-      </c>
-      <c r="E9">
-        <f>VLOOKUP(A9,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>3</v>
+        <v>115</v>
+      </c>
+      <c r="B9">
+        <v>76</v>
+      </c>
+      <c r="D9">
+        <v>39</v>
+      </c>
+      <c r="E9" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
-      <c r="C10" t="s">
-        <v>119</v>
-      </c>
-      <c r="E10">
+      <c r="B10">
+        <v>77</v>
+      </c>
+      <c r="D10">
         <f>VLOOKUP(A10,Hoja3!$F$3:$G$45,2,0)</f>
         <v>5</v>
+      </c>
+      <c r="E10" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
-      <c r="C11" t="s">
-        <v>119</v>
-      </c>
-      <c r="E11">
+      <c r="B11">
+        <v>78</v>
+      </c>
+      <c r="D11">
         <f>VLOOKUP(A11,Hoja3!$F$3:$G$45,2,0)</f>
         <v>6</v>
       </c>
+      <c r="E11" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>121</v>
-      </c>
-      <c r="C12" t="s">
-        <v>116</v>
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>26</v>
       </c>
       <c r="D12">
-        <v>26</v>
+        <f>VLOOKUP(A12,Hoja3!$F$3:$G$45,2,0)</f>
+        <v>7</v>
+      </c>
+      <c r="E12" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" t="s">
-        <v>117</v>
-      </c>
-      <c r="E13">
-        <f>VLOOKUP(A13,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>7</v>
+        <v>135</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>26</v>
+      </c>
+      <c r="E13" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" t="s">
-        <v>117</v>
-      </c>
-      <c r="E14">
-        <f>VLOOKUP(A14,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>8</v>
+        <v>121</v>
+      </c>
+      <c r="B14">
+        <v>79</v>
+      </c>
+      <c r="D14">
+        <v>40</v>
+      </c>
+      <c r="E14" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>91</v>
-      </c>
-      <c r="C15" t="s">
-        <v>122</v>
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <v>27</v>
       </c>
       <c r="D15">
-        <f>VLOOKUP(A15,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>18</v>
+        <f>VLOOKUP(A15,Hoja3!$F$3:$G$45,2,0)</f>
+        <v>8</v>
+      </c>
+      <c r="E15" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" t="s">
-        <v>117</v>
-      </c>
-      <c r="E16">
-        <f>VLOOKUP(A16,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>9</v>
+        <v>136</v>
+      </c>
+      <c r="B16">
+        <v>80</v>
+      </c>
+      <c r="D16">
+        <v>41</v>
+      </c>
+      <c r="E16" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>123</v>
-      </c>
-      <c r="C17" t="s">
-        <v>116</v>
-      </c>
-      <c r="D17">
-        <v>33</v>
+        <v>91</v>
+      </c>
+      <c r="B17">
+        <v>50</v>
+      </c>
+      <c r="C17">
+        <f>VLOOKUP(A17,Hoja3!$C$3:$D$35,2,0)</f>
+        <v>18</v>
+      </c>
+      <c r="E17" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18">
+        <v>28</v>
+      </c>
+      <c r="D18">
+        <f>VLOOKUP(A18,Hoja3!$F$3:$G$45,2,0)</f>
+        <v>9</v>
+      </c>
+      <c r="E18" t="s">
         <v>117</v>
-      </c>
-      <c r="E18">
-        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <v>29</v>
+      </c>
+      <c r="D19">
+        <v>10</v>
+      </c>
+      <c r="E19" t="s">
         <v>117</v>
-      </c>
-      <c r="E19">
-        <f>VLOOKUP(A19,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>124</v>
-      </c>
-      <c r="C20" t="s">
+        <v>123</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20">
+        <v>33</v>
+      </c>
+      <c r="E20" t="s">
         <v>116</v>
-      </c>
-      <c r="D20">
-        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21">
+        <v>30</v>
+      </c>
+      <c r="D21">
+        <f>VLOOKUP(A21,Hoja3!$F$3:$G$45,2,0)</f>
+        <v>11</v>
+      </c>
+      <c r="E21" t="s">
         <v>117</v>
-      </c>
-      <c r="E21">
-        <f>VLOOKUP(A21,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>21</v>
-      </c>
-      <c r="C22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>31</v>
+      </c>
+      <c r="D22">
+        <f>VLOOKUP(A22,Hoja3!$F$3:$G$45,2,0)</f>
+        <v>12</v>
+      </c>
+      <c r="E22" t="s">
         <v>117</v>
-      </c>
-      <c r="E22">
-        <f>VLOOKUP(A22,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23">
-        <f>VLOOKUP(A23,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>29</v>
-      </c>
-      <c r="E23">
-        <f>VLOOKUP(A23,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>14</v>
+        <v>124</v>
+      </c>
+      <c r="B23">
+        <v>7</v>
+      </c>
+      <c r="C23">
+        <v>30</v>
+      </c>
+      <c r="E23" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24">
-        <v>77</v>
-      </c>
-      <c r="D24" t="e">
-        <f>VLOOKUP(A24,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E24">
+        <v>21</v>
+      </c>
+      <c r="B24">
+        <v>32</v>
+      </c>
+      <c r="D24">
         <f>VLOOKUP(A24,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>15</v>
+        <v>13</v>
+      </c>
+      <c r="E24" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>64</v>
-      </c>
-      <c r="C25">
-        <v>4</v>
-      </c>
-      <c r="D25" t="e">
-        <f>VLOOKUP(A25,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E25" t="e">
+        <v>12</v>
+      </c>
+      <c r="B25">
+        <v>33</v>
+      </c>
+      <c r="D25">
         <f>VLOOKUP(A25,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>#N/A</v>
+        <v>14</v>
+      </c>
+      <c r="E25" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26">
-        <v>10</v>
+        <v>23</v>
+      </c>
+      <c r="B26">
+        <v>34</v>
       </c>
       <c r="D26">
-        <f>VLOOKUP(A26,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>31</v>
-      </c>
-      <c r="E26" t="e">
         <f>VLOOKUP(A26,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>#N/A</v>
+        <v>15</v>
+      </c>
+      <c r="E26" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27">
-        <v>78</v>
-      </c>
-      <c r="D27" t="e">
-        <f>VLOOKUP(A27,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E27">
-        <f>VLOOKUP(A27,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>16</v>
+        <v>64</v>
+      </c>
+      <c r="B27">
+        <v>8</v>
+      </c>
+      <c r="E27" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>88</v>
-      </c>
-      <c r="C28">
-        <v>42</v>
-      </c>
-      <c r="D28" t="e">
-        <f>VLOOKUP(A28,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E28" t="e">
-        <f>VLOOKUP(A28,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>#N/A</v>
+        <v>25</v>
+      </c>
+      <c r="B28">
+        <v>35</v>
+      </c>
+      <c r="D28">
+        <v>16</v>
+      </c>
+      <c r="E28" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>24</v>
+      </c>
+      <c r="B29">
+        <v>9</v>
       </c>
       <c r="C29">
-        <v>79</v>
-      </c>
-      <c r="D29" t="e">
-        <f>VLOOKUP(A29,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E29">
-        <f>VLOOKUP(A29,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>17</v>
+        <v>31</v>
+      </c>
+      <c r="E29" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>14</v>
-      </c>
-      <c r="C30">
-        <v>17</v>
+      <c r="A30" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B30">
+        <v>81</v>
       </c>
       <c r="D30">
-        <f>VLOOKUP(A30,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>9</v>
-      </c>
-      <c r="E30">
-        <f>VLOOKUP(A30,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>18</v>
+        <v>45</v>
+      </c>
+      <c r="E30" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>27</v>
-      </c>
-      <c r="C31">
-        <v>16</v>
-      </c>
-      <c r="D31" t="e">
-        <f>VLOOKUP(A31,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E31">
-        <f>VLOOKUP(A31,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>19</v>
+        <v>88</v>
+      </c>
+      <c r="B31">
+        <v>36</v>
+      </c>
+      <c r="D31">
+        <v>17</v>
+      </c>
+      <c r="E31" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>57</v>
-      </c>
-      <c r="C32">
-        <v>48</v>
+        <v>14</v>
+      </c>
+      <c r="B32">
+        <v>37</v>
       </c>
       <c r="D32">
-        <f>VLOOKUP(A32,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>8</v>
-      </c>
-      <c r="E32" t="e">
-        <f>VLOOKUP(A32,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>#N/A</v>
+        <v>18</v>
+      </c>
+      <c r="E32" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>85</v>
+        <v>125</v>
+      </c>
+      <c r="B33">
+        <v>10</v>
       </c>
       <c r="C33">
-        <v>41</v>
-      </c>
-      <c r="D33" t="e">
-        <f>VLOOKUP(A33,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E33" t="e">
-        <f>VLOOKUP(A33,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>#N/A</v>
+        <v>9</v>
+      </c>
+      <c r="E33" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>28</v>
-      </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-      <c r="D34" t="e">
-        <f>VLOOKUP(A34,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E34">
+        <v>27</v>
+      </c>
+      <c r="B34">
+        <v>38</v>
+      </c>
+      <c r="D34">
         <f>VLOOKUP(A34,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="E34" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>92</v>
+        <v>85</v>
+      </c>
+      <c r="B35">
+        <v>72</v>
       </c>
       <c r="C35">
-        <v>49</v>
-      </c>
-      <c r="D35">
-        <f>VLOOKUP(A35,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>1</v>
-      </c>
-      <c r="E35" t="e">
-        <f>VLOOKUP(A35,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>#N/A</v>
+        <v>8</v>
+      </c>
+      <c r="E35" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>75</v>
-      </c>
-      <c r="C36">
-        <v>23</v>
-      </c>
-      <c r="D36" t="e">
-        <f>VLOOKUP(A36,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E36" t="e">
-        <f>VLOOKUP(A36,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>#N/A</v>
+        <v>85</v>
+      </c>
+      <c r="B36">
+        <v>82</v>
+      </c>
+      <c r="D36">
+        <v>42</v>
+      </c>
+      <c r="E36" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>111</v>
-      </c>
-      <c r="C37">
-        <v>50</v>
+        <v>28</v>
+      </c>
+      <c r="B37">
+        <v>39</v>
       </c>
       <c r="D37">
-        <v>15</v>
+        <v>20</v>
+      </c>
+      <c r="E37" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>29</v>
+        <v>126</v>
+      </c>
+      <c r="B38">
+        <v>51</v>
       </c>
       <c r="C38">
-        <v>25</v>
-      </c>
-      <c r="E38">
-        <f>VLOOKUP(A38,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>21</v>
+        <v>1</v>
+      </c>
+      <c r="E38" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>31</v>
-      </c>
-      <c r="C39">
-        <v>35</v>
-      </c>
-      <c r="D39">
-        <f>VLOOKUP(A39,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>16</v>
-      </c>
-      <c r="E39">
-        <f>VLOOKUP(A39,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>22</v>
+        <v>75</v>
+      </c>
+      <c r="B39">
+        <v>52</v>
+      </c>
+      <c r="E39" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>35</v>
-      </c>
-      <c r="C40">
-        <v>81</v>
-      </c>
-      <c r="D40" t="e">
-        <f>VLOOKUP(A40,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E40">
+        <v>29</v>
+      </c>
+      <c r="B40">
+        <v>40</v>
+      </c>
+      <c r="D40">
         <f>VLOOKUP(A40,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>24</v>
+        <v>21</v>
+      </c>
+      <c r="E40" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>33</v>
-      </c>
-      <c r="C41">
-        <v>80</v>
-      </c>
-      <c r="D41" t="e">
-        <f>VLOOKUP(A41,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E41">
-        <f>VLOOKUP(A41,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>23</v>
+        <v>31</v>
+      </c>
+      <c r="B41">
+        <v>41</v>
+      </c>
+      <c r="D41">
+        <v>22</v>
+      </c>
+      <c r="E41" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>37</v>
+        <v>127</v>
+      </c>
+      <c r="B42">
+        <v>11</v>
       </c>
       <c r="C42">
-        <v>32</v>
-      </c>
-      <c r="D42">
-        <f>VLOOKUP(A42,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>32</v>
-      </c>
-      <c r="E42" t="e">
-        <f>VLOOKUP(A42,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>#N/A</v>
+        <v>16</v>
+      </c>
+      <c r="E42" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>38</v>
+        <v>111</v>
+      </c>
+      <c r="B43">
+        <v>12</v>
       </c>
       <c r="C43">
-        <v>82</v>
-      </c>
-      <c r="D43" t="e">
-        <f>VLOOKUP(A43,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E43">
-        <f>VLOOKUP(A43,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>25</v>
+        <v>15</v>
+      </c>
+      <c r="E43" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>39</v>
+        <v>37</v>
+      </c>
+      <c r="B44">
+        <v>13</v>
       </c>
       <c r="C44">
-        <v>15</v>
-      </c>
-      <c r="D44" t="e">
-        <f>VLOOKUP(A44,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E44">
-        <f>VLOOKUP(A44,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>26</v>
+        <v>32</v>
+      </c>
+      <c r="E44" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>3</v>
-      </c>
-      <c r="C45">
-        <v>52</v>
+        <v>38</v>
+      </c>
+      <c r="B45">
+        <v>42</v>
       </c>
       <c r="D45">
-        <f>VLOOKUP(A45,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>22</v>
-      </c>
-      <c r="E45" t="e">
-        <f>VLOOKUP(A45,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>#N/A</v>
+        <v>25</v>
+      </c>
+      <c r="E45" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>59</v>
-      </c>
-      <c r="C46">
-        <v>53</v>
+        <v>39</v>
+      </c>
+      <c r="B46">
+        <v>43</v>
       </c>
       <c r="D46">
-        <f>VLOOKUP(A46,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>23</v>
-      </c>
-      <c r="E46" t="e">
-        <f>VLOOKUP(A46,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>#N/A</v>
+        <v>26</v>
+      </c>
+      <c r="E46" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>40</v>
+        <v>3</v>
+      </c>
+      <c r="B47">
+        <v>6</v>
       </c>
       <c r="C47">
-        <v>26</v>
-      </c>
-      <c r="D47">
-        <f>VLOOKUP(A47,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>24</v>
-      </c>
-      <c r="E47">
-        <f>VLOOKUP(A47,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>27</v>
+        <v>22</v>
+      </c>
+      <c r="E47" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>77</v>
-      </c>
-      <c r="C48">
-        <v>24</v>
-      </c>
-      <c r="D48" t="e">
-        <f>VLOOKUP(A48,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E48" t="e">
-        <f>VLOOKUP(A48,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>#N/A</v>
+        <v>40</v>
+      </c>
+      <c r="B48">
+        <v>45</v>
+      </c>
+      <c r="D48">
+        <v>27</v>
+      </c>
+      <c r="E48" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>42</v>
+        <v>130</v>
+      </c>
+      <c r="B49">
+        <v>14</v>
       </c>
       <c r="C49">
-        <v>27</v>
-      </c>
-      <c r="D49" t="e">
-        <f>VLOOKUP(A49,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E49">
-        <f>VLOOKUP(A49,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>28</v>
+        <v>24</v>
+      </c>
+      <c r="E49" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>43</v>
-      </c>
-      <c r="C50">
-        <v>83</v>
-      </c>
-      <c r="D50" t="e">
-        <f>VLOOKUP(A50,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E50">
-        <f>VLOOKUP(A50,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>29</v>
+        <v>77</v>
+      </c>
+      <c r="B50">
+        <v>53</v>
+      </c>
+      <c r="E50" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>44</v>
-      </c>
-      <c r="C51">
-        <v>84</v>
-      </c>
-      <c r="D51" t="e">
-        <f>VLOOKUP(A51,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E51">
-        <f>VLOOKUP(A51,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>30</v>
+        <v>42</v>
+      </c>
+      <c r="B51">
+        <v>22</v>
+      </c>
+      <c r="D51">
+        <v>28</v>
+      </c>
+      <c r="E51" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>45</v>
-      </c>
-      <c r="C52">
-        <v>85</v>
-      </c>
-      <c r="D52" t="e">
-        <f>VLOOKUP(A52,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E52">
-        <f>VLOOKUP(A52,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>31</v>
+        <v>137</v>
+      </c>
+      <c r="B52">
+        <v>44</v>
+      </c>
+      <c r="D52">
+        <v>43</v>
+      </c>
+      <c r="E52" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>79</v>
+        <v>129</v>
+      </c>
+      <c r="B53">
+        <v>15</v>
       </c>
       <c r="C53">
-        <v>31</v>
-      </c>
-      <c r="D53" t="e">
-        <f>VLOOKUP(A53,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E53" t="e">
-        <f>VLOOKUP(A53,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>#N/A</v>
+        <v>23</v>
+      </c>
+      <c r="E53" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>78</v>
-      </c>
-      <c r="C54">
+        <v>43</v>
+      </c>
+      <c r="B54">
+        <v>83</v>
+      </c>
+      <c r="D54">
         <v>29</v>
       </c>
-      <c r="D54" t="e">
-        <f>VLOOKUP(A54,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E54" t="e">
-        <f>VLOOKUP(A54,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>#N/A</v>
+      <c r="E54" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
+        <v>44</v>
+      </c>
+      <c r="B55">
         <v>84</v>
       </c>
-      <c r="C55">
-        <v>39</v>
-      </c>
-      <c r="D55" t="e">
-        <f>VLOOKUP(A55,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E55" t="e">
-        <f>VLOOKUP(A55,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>#N/A</v>
+      <c r="D55">
+        <v>30</v>
+      </c>
+      <c r="E55" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>66</v>
-      </c>
-      <c r="C56">
-        <v>7</v>
-      </c>
-      <c r="D56" t="e">
-        <f>VLOOKUP(A56,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E56" t="e">
-        <f>VLOOKUP(A56,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>#N/A</v>
+        <v>45</v>
+      </c>
+      <c r="B56">
+        <v>85</v>
+      </c>
+      <c r="D56">
+        <v>31</v>
+      </c>
+      <c r="E56" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>65</v>
-      </c>
-      <c r="C57">
-        <v>5</v>
-      </c>
-      <c r="D57" t="e">
-        <f>VLOOKUP(A57,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E57" t="e">
-        <f>VLOOKUP(A57,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>#N/A</v>
+        <v>79</v>
+      </c>
+      <c r="B57">
+        <v>54</v>
+      </c>
+      <c r="E57" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>70</v>
-      </c>
-      <c r="C58">
-        <v>12</v>
-      </c>
-      <c r="D58" t="e">
-        <f>VLOOKUP(A58,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E58" t="e">
-        <f>VLOOKUP(A58,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>#N/A</v>
+        <v>78</v>
+      </c>
+      <c r="B58">
+        <v>55</v>
+      </c>
+      <c r="E58" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>68</v>
-      </c>
-      <c r="C59">
-        <v>9</v>
-      </c>
-      <c r="D59" t="e">
-        <f>VLOOKUP(A59,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E59" t="e">
-        <f>VLOOKUP(A59,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>#N/A</v>
+        <v>84</v>
+      </c>
+      <c r="B59">
+        <v>56</v>
+      </c>
+      <c r="E59" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>72</v>
-      </c>
-      <c r="C60">
-        <v>14</v>
-      </c>
-      <c r="D60" t="e">
-        <f>VLOOKUP(A60,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E60" t="e">
-        <f>VLOOKUP(A60,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>#N/A</v>
+        <v>66</v>
+      </c>
+      <c r="B60">
+        <v>57</v>
+      </c>
+      <c r="E60" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>93</v>
-      </c>
-      <c r="C61">
-        <v>55</v>
-      </c>
-      <c r="D61">
-        <f>VLOOKUP(A61,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>2</v>
-      </c>
-      <c r="E61" t="e">
-        <f>VLOOKUP(A61,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>#N/A</v>
+        <v>65</v>
+      </c>
+      <c r="B61">
+        <v>58</v>
+      </c>
+      <c r="E61" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>18</v>
-      </c>
-      <c r="C62">
-        <v>56</v>
-      </c>
-      <c r="D62">
-        <f>VLOOKUP(A62,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>28</v>
-      </c>
-      <c r="E62">
-        <f>VLOOKUP(A62,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>32</v>
+        <v>70</v>
+      </c>
+      <c r="B62">
+        <v>59</v>
+      </c>
+      <c r="E62" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>80</v>
-      </c>
-      <c r="C63">
-        <v>34</v>
-      </c>
-      <c r="D63" t="e">
-        <f>VLOOKUP(A63,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E63" t="e">
-        <f>VLOOKUP(A63,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>#N/A</v>
+        <v>68</v>
+      </c>
+      <c r="B63">
+        <v>60</v>
+      </c>
+      <c r="E63" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>94</v>
-      </c>
-      <c r="C64">
-        <v>57</v>
-      </c>
-      <c r="D64">
-        <f>VLOOKUP(A64,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>27</v>
-      </c>
-      <c r="E64" t="e">
-        <f>VLOOKUP(A64,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>#N/A</v>
+        <v>72</v>
+      </c>
+      <c r="B64">
+        <v>61</v>
+      </c>
+      <c r="E64" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>67</v>
-      </c>
-      <c r="C65">
-        <v>8</v>
-      </c>
-      <c r="D65" t="e">
-        <f>VLOOKUP(A65,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E65" t="e">
-        <f>VLOOKUP(A65,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>#N/A</v>
+        <v>93</v>
+      </c>
+      <c r="B65">
+        <v>62</v>
+      </c>
+      <c r="E65" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>95</v>
+        <v>18</v>
+      </c>
+      <c r="B66">
+        <v>16</v>
       </c>
       <c r="C66">
-        <v>58</v>
-      </c>
-      <c r="D66">
-        <f>VLOOKUP(A66,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>13</v>
-      </c>
-      <c r="E66" t="e">
-        <f>VLOOKUP(A66,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>#N/A</v>
+        <v>28</v>
+      </c>
+      <c r="E66" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>96</v>
-      </c>
-      <c r="C67">
-        <v>59</v>
+        <v>18</v>
+      </c>
+      <c r="B67">
+        <v>46</v>
       </c>
       <c r="D67">
-        <f>VLOOKUP(A67,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>7</v>
-      </c>
-      <c r="E67" t="e">
-        <f>VLOOKUP(A67,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>#N/A</v>
+        <v>32</v>
+      </c>
+      <c r="E67" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>97</v>
-      </c>
-      <c r="C68">
-        <v>60</v>
-      </c>
-      <c r="D68">
-        <f>VLOOKUP(A68,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>14</v>
-      </c>
-      <c r="E68" t="e">
-        <f>VLOOKUP(A68,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>#N/A</v>
+        <v>80</v>
+      </c>
+      <c r="B68">
+        <v>63</v>
+      </c>
+      <c r="E68" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>47</v>
+        <v>67</v>
+      </c>
+      <c r="B69">
+        <v>92</v>
       </c>
       <c r="C69">
-        <v>87</v>
-      </c>
-      <c r="D69" t="e">
-        <f>VLOOKUP(A69,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E69">
-        <f>VLOOKUP(A69,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>33</v>
+        <v>27</v>
+      </c>
+      <c r="E69" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>62</v>
+        <v>95</v>
+      </c>
+      <c r="B70">
+        <v>64</v>
       </c>
       <c r="C70">
-        <v>2</v>
-      </c>
-      <c r="D70">
-        <f>VLOOKUP(A70,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>10</v>
-      </c>
-      <c r="E70" t="e">
-        <f>VLOOKUP(A70,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>#N/A</v>
+        <v>13</v>
+      </c>
+      <c r="E70" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>63</v>
+        <v>96</v>
+      </c>
+      <c r="B71">
+        <v>65</v>
       </c>
       <c r="C71">
-        <v>3</v>
-      </c>
-      <c r="D71">
-        <f>VLOOKUP(A71,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>11</v>
-      </c>
-      <c r="E71" t="e">
-        <f>VLOOKUP(A71,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>#N/A</v>
+        <v>7</v>
+      </c>
+      <c r="E71" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>36</v>
+        <v>97</v>
+      </c>
+      <c r="B72">
+        <v>66</v>
       </c>
       <c r="C72">
-        <v>61</v>
-      </c>
-      <c r="D72">
-        <f>VLOOKUP(A72,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>4</v>
-      </c>
-      <c r="E72" t="e">
-        <f>VLOOKUP(A72,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>#N/A</v>
+        <v>14</v>
+      </c>
+      <c r="E72" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>82</v>
-      </c>
-      <c r="C73">
-        <v>37</v>
-      </c>
-      <c r="D73" t="e">
-        <f>VLOOKUP(A73,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E73" t="e">
-        <f>VLOOKUP(A73,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>#N/A</v>
+        <v>47</v>
+      </c>
+      <c r="B73">
+        <v>86</v>
+      </c>
+      <c r="D73">
+        <v>33</v>
+      </c>
+      <c r="E73" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>83</v>
+        <v>62</v>
+      </c>
+      <c r="B74">
+        <v>67</v>
       </c>
       <c r="C74">
-        <v>38</v>
-      </c>
-      <c r="D74">
-        <f>VLOOKUP(A74,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>6</v>
-      </c>
-      <c r="E74" t="e">
-        <f>VLOOKUP(A74,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>#N/A</v>
+        <v>10</v>
+      </c>
+      <c r="E74" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>60</v>
+        <v>63</v>
+      </c>
+      <c r="B75">
+        <v>68</v>
       </c>
       <c r="C75">
-        <v>88</v>
-      </c>
-      <c r="D75" t="e">
-        <f>VLOOKUP(A75,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E75">
-        <f>VLOOKUP(A75,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>34</v>
+        <v>11</v>
+      </c>
+      <c r="E75" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>98</v>
+        <v>82</v>
+      </c>
+      <c r="B76">
+        <v>17</v>
       </c>
       <c r="C76">
-        <v>63</v>
-      </c>
-      <c r="D76">
-        <f>VLOOKUP(A76,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>19</v>
-      </c>
-      <c r="E76" t="e">
-        <f>VLOOKUP(A76,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>#N/A</v>
+        <v>4</v>
+      </c>
+      <c r="E76" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>99</v>
-      </c>
-      <c r="C77">
-        <v>64</v>
+        <v>138</v>
+      </c>
+      <c r="B77">
+        <v>47</v>
       </c>
       <c r="D77">
-        <f>VLOOKUP(A77,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>20</v>
-      </c>
-      <c r="E77" t="e">
-        <f>VLOOKUP(A77,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>#N/A</v>
+        <v>24</v>
+      </c>
+      <c r="E77" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>49</v>
-      </c>
-      <c r="C78">
-        <v>65</v>
+        <v>83</v>
+      </c>
+      <c r="B78">
+        <v>48</v>
       </c>
       <c r="D78">
-        <f>VLOOKUP(A78,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>5</v>
-      </c>
-      <c r="E78">
-        <f>VLOOKUP(A78,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>35</v>
+        <v>23</v>
+      </c>
+      <c r="E78" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>100</v>
-      </c>
-      <c r="C79">
-        <v>66</v>
+        <v>60</v>
+      </c>
+      <c r="B79">
+        <v>87</v>
       </c>
       <c r="D79">
-        <f>VLOOKUP(A79,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>21</v>
-      </c>
-      <c r="E79" t="e">
-        <f>VLOOKUP(A79,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>#N/A</v>
+        <v>34</v>
+      </c>
+      <c r="E79" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>101</v>
+        <v>132</v>
+      </c>
+      <c r="B80">
+        <v>18</v>
       </c>
       <c r="C80">
-        <v>67</v>
-      </c>
-      <c r="D80">
-        <f>VLOOKUP(A80,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>12</v>
-      </c>
-      <c r="E80" t="e">
-        <f>VLOOKUP(A80,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>#N/A</v>
+        <v>6</v>
+      </c>
+      <c r="E80" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>50</v>
+        <v>98</v>
+      </c>
+      <c r="B81">
+        <v>69</v>
       </c>
       <c r="C81">
-        <v>21</v>
-      </c>
-      <c r="D81" t="e">
-        <f>VLOOKUP(A81,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E81">
-        <f>VLOOKUP(A81,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>36</v>
+        <v>19</v>
+      </c>
+      <c r="E81" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>74</v>
+        <v>99</v>
+      </c>
+      <c r="B82">
+        <v>70</v>
       </c>
       <c r="C82">
-        <v>22</v>
-      </c>
-      <c r="D82" t="e">
-        <f>VLOOKUP(A82,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E82" t="e">
-        <f>VLOOKUP(A82,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>#N/A</v>
+        <v>20</v>
+      </c>
+      <c r="E82" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>81</v>
-      </c>
-      <c r="C83">
-        <v>36</v>
+        <v>49</v>
+      </c>
+      <c r="B83">
+        <v>49</v>
       </c>
       <c r="D83">
-        <f>VLOOKUP(A83,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>3</v>
-      </c>
-      <c r="E83" t="e">
-        <f>VLOOKUP(A83,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>#N/A</v>
+        <v>35</v>
+      </c>
+      <c r="E83" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>51</v>
+        <v>100</v>
+      </c>
+      <c r="B84">
+        <v>71</v>
       </c>
       <c r="C84">
-        <v>90</v>
-      </c>
-      <c r="D84" t="e">
-        <f>VLOOKUP(A84,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E84">
-        <f>VLOOKUP(A84,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>37</v>
+        <v>21</v>
+      </c>
+      <c r="E84" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>52</v>
+        <v>133</v>
+      </c>
+      <c r="B85">
+        <v>19</v>
       </c>
       <c r="C85">
-        <v>91</v>
-      </c>
-      <c r="D85" t="e">
-        <f>VLOOKUP(A85,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E85">
-        <f>VLOOKUP(A85,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>38</v>
+        <v>5</v>
+      </c>
+      <c r="E85" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>53</v>
+        <v>101</v>
+      </c>
+      <c r="B86">
+        <v>73</v>
       </c>
       <c r="C86">
-        <v>92</v>
-      </c>
-      <c r="D86" t="e">
-        <f>VLOOKUP(A86,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E86">
-        <f>VLOOKUP(A86,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>39</v>
+        <v>12</v>
+      </c>
+      <c r="E86" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>54</v>
-      </c>
-      <c r="C87">
-        <v>93</v>
-      </c>
-      <c r="D87" t="e">
-        <f>VLOOKUP(A87,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E87">
-        <f>VLOOKUP(A87,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>40</v>
+        <v>50</v>
+      </c>
+      <c r="B87">
+        <v>88</v>
+      </c>
+      <c r="D87">
+        <v>36</v>
+      </c>
+      <c r="E87" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>55</v>
-      </c>
-      <c r="C88">
-        <v>94</v>
-      </c>
-      <c r="D88" t="e">
-        <f>VLOOKUP(A88,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E88">
-        <f>VLOOKUP(A88,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>41</v>
+        <v>74</v>
+      </c>
+      <c r="B88">
+        <v>89</v>
+      </c>
+      <c r="D88">
+        <v>44</v>
+      </c>
+      <c r="E88" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>71</v>
+        <v>81</v>
+      </c>
+      <c r="B89">
+        <v>20</v>
       </c>
       <c r="C89">
-        <v>13</v>
-      </c>
-      <c r="D89" t="e">
-        <f>VLOOKUP(A89,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E89" t="e">
-        <f>VLOOKUP(A89,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>#N/A</v>
+        <v>3</v>
+      </c>
+      <c r="E89" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>56</v>
-      </c>
-      <c r="C90">
-        <v>95</v>
-      </c>
-      <c r="D90" t="e">
-        <f>VLOOKUP(A90,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E90">
-        <f>VLOOKUP(A90,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>42</v>
+        <v>51</v>
+      </c>
+      <c r="B90">
+        <v>90</v>
+      </c>
+      <c r="D90">
+        <v>37</v>
+      </c>
+      <c r="E90" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>58</v>
-      </c>
-      <c r="C91">
-        <v>96</v>
-      </c>
-      <c r="D91" t="e">
-        <f>VLOOKUP(A91,Hoja3!$C$3:$D$35,2,0)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="E91">
-        <f>VLOOKUP(A91,Hoja3!$F$3:$G$45,2,0)</f>
-        <v>43</v>
+        <v>52</v>
+      </c>
+      <c r="B91">
+        <v>91</v>
+      </c>
+      <c r="D91">
+        <v>38</v>
+      </c>
+      <c r="E91" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>114</v>
+      </c>
+      <c r="B92">
+        <v>74</v>
+      </c>
+      <c r="C92">
+        <v>17</v>
+      </c>
+      <c r="E92" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>71</v>
+      </c>
+      <c r="B93">
+        <v>21</v>
+      </c>
+      <c r="E93" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C1" xr:uid="{1E37CA9D-18F6-44B6-95D3-67168C9C737D}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C97">
-      <sortCondition ref="A1"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93EE3A1B-1DBE-431E-8039-9E230BF0B6D2}">
-  <dimension ref="C2:G45"/>
+  <dimension ref="C2:G47"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="A1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2759,6 +2744,22 @@
         <v>43</v>
       </c>
     </row>
+    <row r="46" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="F46" t="s">
+        <v>74</v>
+      </c>
+      <c r="G46">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="47" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="F47" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G47">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2769,8 +2770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DF4F5D-4055-42C5-AAB7-659A5EC57DCD}">
   <dimension ref="B2:K47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>